<commit_message>
Added food survey app
</commit_message>
<xml_diff>
--- a/fp1/survey_responses/food_recommendation_survey_results.xlsx
+++ b/fp1/survey_responses/food_recommendation_survey_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isbhydmoh-my.sharepoint.com/personal/kanishk_gupta_ampba2024s_isb_edu/Documents/Desktop/ISB/github_codes/ampba_24_group18_term2/fp1/survey_responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{0BB1D911-D205-4457-8524-AEF5AD3534F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADDF160B-02AB-4BFE-88C8-CFB06D5201B2}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{0BB1D911-D205-4457-8524-AEF5AD3534F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BE490E0-E5C7-437C-8DC7-4150D02C80E7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,6 +516,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O5" totalsRowShown="0">
   <autoFilter ref="A1:O5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -1076,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFD9D92-F606-4226-B0D4-F64EC46C2DB4}">
   <dimension ref="A1:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2036,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7F2100-F3CC-48DE-9595-BE127D50657B}">
   <dimension ref="C2:K1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView topLeftCell="A1000" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E1023"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2046,7 +2050,7 @@
     <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.08984375" customWidth="1"/>
     <col min="7" max="7" width="14.36328125" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="8" max="8" width="34.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1796875" customWidth="1"/>

</xml_diff>